<commit_message>
add inv et order in WeeklyReport
</commit_message>
<xml_diff>
--- a/templates/Planning.xlsx
+++ b/templates/Planning.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22527"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\GPM2\templates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\GPM\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F63B458-B84E-4DC8-9244-8CB4F4AA858E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B71E09A9-13DE-4326-8187-7C79284B0101}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-5460" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="36255" yWindow="-4155" windowWidth="26985" windowHeight="16215" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Worksheet" sheetId="1" r:id="rId1"/>
@@ -716,8 +716,8 @@
     </row>
     <row r="44" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C44" t="str">
-        <f>CONCATENATE("INSERT INTO `planning_users`(`id_user`, `dateplanned`, `quantity`, `type`) VALUES ('",$J29,"', '",TEXT(C$6,"yyyy-mm-dd"),"', '",C7,"', '",C18,"') ON DUPLICATE KEY UPDATE quantity='",C7,"', type='",C18,"';")</f>
-        <v>INSERT INTO `planning_users`(`id_user`, `dateplanned`, `quantity`, `type`) VALUES ('', '1900-01-00', '', '') ON DUPLICATE KEY UPDATE quantity='', type='';</v>
+        <f>CONCATENATE("INSERT INTO `planning_users`(`id_user`, `dateplanned`, `quantity`, `type`) VALUES ('",$J29,"', '",TEXT(C$6,"yyyy-mm-dd"),"', '",C7,"', '",C18,"') ON DUPLICATE KEY UPDATE quantity='",C7,"', type='",C18,"';"," UPDATE planning_modif set id_validator=-1 where id_user='",$J29,"' AND date(datemodif)='",TEXT(C$6,"yyyy-mm-dd"),"';")</f>
+        <v>INSERT INTO `planning_users`(`id_user`, `dateplanned`, `quantity`, `type`) VALUES ('', '1900-01-00', '', '') ON DUPLICATE KEY UPDATE quantity='', type=''; UPDATE planning_modif set id_validator=-1 where id_user='' AND date(datemodif)='1900-01-00';</v>
       </c>
     </row>
   </sheetData>

</xml_diff>